<commit_message>
Aggiornato il file Excel ESERCIZIO_M2-1-1_dati
</commit_message>
<xml_diff>
--- a/ESERCIZIO_M2-1-1_dati.xlsx
+++ b/ESERCIZIO_M2-1-1_dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/576cc10a439d64a5/Desktop/Epicode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{570F9955-4413-4EC3-8BC2-9CC782817029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{570F9955-4413-4EC3-8BC2-9CC782817029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAEF6F16-BE7E-41C5-BCE2-83C1D695F519}"/>
   <bookViews>
-    <workbookView xWindow="36495" yWindow="4095" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assoluti_Iva" sheetId="1" r:id="rId1"/>
@@ -65,8 +65,54 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E1476664-F5C1-4AEB-8953-E52DA86991B9}</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{E1476664-F5C1-4AEB-8953-E52DA86991B9}">
+      <text>
+        <t>[Commento in thread]
+La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
+Commento:
+ Totale IVA Inclusa = Imponibile + IVA
+Totale IVA Inclusa = Imponible * (1+0,20)
+IVA = Totale IVA Inclusa * 20/(100+20)
+Prezzo senza IVA = (100*prezzo con IVA)/(100+20)
+L’IVA = Prezzo con IVA - Imponibile
+L’IVA = (120*prezzo con IVA - 100*prezzo con IVA)/120
+L’IVA = 20*prezzo con IVA/120</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="580">
   <si>
     <t>MONITOR</t>
   </si>
@@ -1793,13 +1839,19 @@
     <t>buono</t>
   </si>
   <si>
-    <t>CERCAVERT Formula</t>
+    <t>CONCAT</t>
   </si>
   <si>
-    <t>SE Formula</t>
+    <t>IVA</t>
   </si>
   <si>
-    <t xml:space="preserve">Totale fatturato </t>
+    <t>PIU.SE Formula</t>
+  </si>
+  <si>
+    <t>CERCA.VERT Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totale fatturato  </t>
   </si>
 </sst>
 </file>
@@ -1811,9 +1863,9 @@
     <numFmt numFmtId="165" formatCode="_-[$€-410]\ * #,##0.00_-;\-[$€-410]\ * #,##0.00_-;_-[$€-410]\ * &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-803]_-;\-* #,##0.00\ [$€-803]_-;_-* &quot;-&quot;??\ [$€-803]_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="#,##0.00\ [$€-410];\-#,##0.00\ [$€-410]"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ [$€-410];\-#,##0.00\ [$€-410]"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1859,6 +1911,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1919,7 +1977,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1966,6 +2024,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Belacurencu Alexandra" id="{132E072E-8370-47E3-941E-08CBACEA083A}" userId="576cc10a439d64a5" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2191,13 +2255,27 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D2" dT="2024-12-12T08:01:03.98" personId="{132E072E-8370-47E3-941E-08CBACEA083A}" id="{E1476664-F5C1-4AEB-8953-E52DA86991B9}">
+    <text xml:space="preserve"> Totale IVA Inclusa = Imponibile + IVA
+Totale IVA Inclusa = Imponible * (1+0,20)
+IVA = Totale IVA Inclusa * 20/(100+20)
+Prezzo senza IVA = (100*prezzo con IVA)/(100+20)
+L’IVA = Prezzo con IVA - Imponibile
+L’IVA = (120*prezzo con IVA - 100*prezzo con IVA)/120
+L’IVA = 20*prezzo con IVA/120</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2222,8 +2300,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>575</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="3"/>
       <c r="H1" s="4"/>
@@ -34033,6 +34115,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -34041,7 +34124,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34065,7 +34148,7 @@
         <v>485</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
@@ -34102,8 +34185,8 @@
       <c r="B2" s="7">
         <v>40</v>
       </c>
-      <c r="C2" s="7" t="str">
-        <f>IF(B2=0,"respinto",IF(B2=40,"sufficiente",IF(B2=60,"discreto",IF(B2=70,"buono"," "))))</f>
+      <c r="C2" s="7" t="str" cm="1">
+        <f t="array" ref="C2">_xlfn.IFS(B2=0,"respinto",B2=40,"sufficiente",B2=60,"discreto",B2=70,"buono")</f>
         <v>sufficiente</v>
       </c>
       <c r="D2" s="8"/>
@@ -34141,8 +34224,8 @@
       <c r="B3" s="7">
         <v>60</v>
       </c>
-      <c r="C3" s="7" t="str">
-        <f t="shared" ref="C3:C8" si="0">IF(B3=0,"respinto",IF(B3=40,"sufficiente",IF(B3=60,"discreto",IF(B3=70,"buono"," "))))</f>
+      <c r="C3" s="7" t="str" cm="1">
+        <f t="array" ref="C3">_xlfn.IFS(B3=0,"respinto",B3=40,"sufficiente",B3=60,"discreto",B3=70,"buono")</f>
         <v>discreto</v>
       </c>
       <c r="E3" s="8">
@@ -34179,8 +34262,8 @@
       <c r="B4" s="7">
         <v>60</v>
       </c>
-      <c r="C4" s="7" t="str">
-        <f>IF(B4=0,"respinto",IF(B4=40,"sufficiente",IF(B4=60,"discreto",IF(B4=70,"buono"," "))))</f>
+      <c r="C4" s="7" t="str" cm="1">
+        <f t="array" ref="C4">_xlfn.IFS(B4=0,"respinto",B4=40,"sufficiente",B4=60,"discreto",B4=70,"buono")</f>
         <v>discreto</v>
       </c>
       <c r="E4" s="8">
@@ -34217,8 +34300,8 @@
       <c r="B5" s="7">
         <v>40</v>
       </c>
-      <c r="C5" s="7" t="str">
-        <f t="shared" si="0"/>
+      <c r="C5" s="7" t="str" cm="1">
+        <f t="array" ref="C5">_xlfn.IFS(B5=0,"respinto",B5=40,"sufficiente",B5=60,"discreto",B5=70,"buono")</f>
         <v>sufficiente</v>
       </c>
       <c r="E5" s="8">
@@ -34255,8 +34338,8 @@
       <c r="B6" s="7">
         <v>70</v>
       </c>
-      <c r="C6" s="7" t="str">
-        <f t="shared" si="0"/>
+      <c r="C6" s="7" t="str" cm="1">
+        <f t="array" ref="C6">_xlfn.IFS(B6=0,"respinto",B6=40,"sufficiente",B6=60,"discreto",B6=70,"buono")</f>
         <v>buono</v>
       </c>
       <c r="E6" s="8"/>
@@ -34289,8 +34372,8 @@
       <c r="B7" s="7">
         <v>0</v>
       </c>
-      <c r="C7" s="7" t="str">
-        <f t="shared" si="0"/>
+      <c r="C7" s="7" t="str" cm="1">
+        <f t="array" ref="C7">_xlfn.IFS(B7=0,"respinto",B7=40,"sufficiente",B7=60,"discreto",B7=70,"buono")</f>
         <v>respinto</v>
       </c>
       <c r="E7" s="8"/>
@@ -34324,7 +34407,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C3:C8" si="0">IF(B8=0,"respinto",IF(B8=40,"sufficiente",IF(B8=60,"discreto",IF(B8=70,"buono"," "))))</f>
         <v>respinto</v>
       </c>
       <c r="E8" s="8"/>
@@ -34408,7 +34491,7 @@
         <v>485</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -61994,7 +62077,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -62032,7 +62115,7 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -62102,7 +62185,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="16">
-        <f t="shared" ref="I3:I7" si="1">SUMIFS($D$2:$D$80, $C$2:$C$80, G3)</f>
+        <f t="shared" ref="I3:I5" si="1">SUMIFS($D$2:$D$80, $C$2:$C$80, G3)</f>
         <v>30860</v>
       </c>
     </row>

</xml_diff>